<commit_message>
final check tranche 2 nulmeting
</commit_message>
<xml_diff>
--- a/VIPP/regeling_2/VIPP Nulmeting Tranche 2.xlsx
+++ b/VIPP/regeling_2/VIPP Nulmeting Tranche 2.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\NL Healthcare Digital\CBI Services\Clinics\ad-hoc_analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/git/PROJECT-BABYLON/VIPP/regeling_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10770" windowHeight="10590"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="26780" windowHeight="22660"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="174">
   <si>
     <t>Wat voor type zorginstelling is uw organisatie?</t>
   </si>
@@ -569,6 +575,9 @@
   <si>
     <t>Clinics kan wel digitaal aanleveren maar heeft geen toegang tot LSP.
 NL Healthcare Clinics heeft herhaaldelijk toegang gevraagd tot het LSP via VZVZ. Tot op heden is daar geen gehoor aangegeven, en is het standpunt van VZVZ dat Clinics 'buiten de doelgroep valt'</t>
+  </si>
+  <si>
+    <t>Sectra</t>
   </si>
 </sst>
 </file>
@@ -673,7 +682,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -953,21 +962,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D125" sqref="D125:D126"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48.1640625" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -976,7 +985,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -989,7 +998,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1004,7 +1013,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1019,7 +1028,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1034,7 +1043,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1045,13 +1054,13 @@
         <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1066,7 +1075,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1081,7 +1090,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1096,7 +1105,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1111,7 +1120,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1126,7 +1135,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1141,7 +1150,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1156,7 +1165,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1171,7 +1180,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -1179,7 +1188,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>15</v>
       </c>
@@ -1193,7 +1202,7 @@
         <v>20063</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>16</v>
       </c>
@@ -1205,7 +1214,7 @@
         <v>19283</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>17</v>
       </c>
@@ -1219,7 +1228,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>18</v>
       </c>
@@ -1231,7 +1240,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -1239,7 +1248,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>19</v>
       </c>
@@ -1249,7 +1258,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>55</v>
@@ -1259,7 +1268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>56</v>
@@ -1269,7 +1278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>57</v>
@@ -1279,7 +1288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>58</v>
@@ -1289,7 +1298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>59</v>
@@ -1299,7 +1308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>60</v>
@@ -1309,7 +1318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>61</v>
@@ -1319,7 +1328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>62</v>
@@ -1329,7 +1338,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>63</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>64</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>65</v>
       </c>
@@ -1353,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
         <v>66</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>67</v>
       </c>
@@ -1369,7 +1378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>68</v>
       </c>
@@ -1377,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>69</v>
       </c>
@@ -1385,7 +1394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="2" t="s">
         <v>70</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>71</v>
       </c>
@@ -1401,7 +1410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>72</v>
       </c>
@@ -1409,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>73</v>
       </c>
@@ -1417,7 +1426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>74</v>
       </c>
@@ -1425,7 +1434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" s="2" t="s">
         <v>75</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>76</v>
       </c>
@@ -1441,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
         <v>77</v>
       </c>
@@ -1449,7 +1458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>78</v>
       </c>
@@ -1457,7 +1466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
         <v>79</v>
@@ -1467,7 +1476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
         <v>80</v>
@@ -1477,7 +1486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>20</v>
       </c>
@@ -1489,7 +1498,7 @@
       </c>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
         <v>82</v>
@@ -1499,7 +1508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
         <v>83</v>
@@ -1509,7 +1518,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
         <v>84</v>
@@ -1519,7 +1528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
         <v>85</v>
@@ -1529,7 +1538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>86</v>
@@ -1539,7 +1548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>21</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>22</v>
       </c>
@@ -1563,7 +1572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>23</v>
       </c>
@@ -1577,7 +1586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>24</v>
       </c>
@@ -1591,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>25</v>
       </c>
@@ -1605,7 +1614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>26</v>
       </c>
@@ -1617,7 +1626,7 @@
       </c>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>27</v>
       </c>
@@ -1629,7 +1638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>28</v>
       </c>
@@ -1641,7 +1650,7 @@
       </c>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>29</v>
       </c>
@@ -1659,7 +1668,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>30</v>
       </c>
@@ -1675,7 +1684,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>31</v>
       </c>
@@ -1695,7 +1704,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>32</v>
       </c>
@@ -1711,7 +1720,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>33</v>
       </c>
@@ -1729,7 +1738,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>34</v>
       </c>
@@ -1745,7 +1754,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>35</v>
       </c>
@@ -1761,7 +1770,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>36</v>
       </c>
@@ -1781,7 +1790,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>37</v>
       </c>
@@ -1799,7 +1808,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>38</v>
       </c>
@@ -1819,7 +1828,7 @@
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>39</v>
       </c>
@@ -1839,7 +1848,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>40</v>
       </c>
@@ -1855,7 +1864,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>154</v>
       </c>
@@ -1867,7 +1876,7 @@
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
     </row>
-    <row r="79" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>41</v>
       </c>
@@ -1887,7 +1896,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>42</v>
       </c>
@@ -1907,7 +1916,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>43</v>
       </c>
@@ -1924,7 +1933,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>44</v>
       </c>
@@ -1941,7 +1950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="150" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>45</v>
       </c>
@@ -1956,7 +1965,7 @@
       </c>
       <c r="E83" s="2"/>
     </row>
-    <row r="84" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>46</v>
       </c>
@@ -1969,7 +1978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>47</v>
       </c>
@@ -1982,7 +1991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>48</v>
       </c>
@@ -1995,7 +2004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>49</v>
       </c>
@@ -2010,7 +2019,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>50</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>51</v>
       </c>
@@ -2036,7 +2045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>52</v>
       </c>
@@ -2049,7 +2058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>53</v>
       </c>
@@ -2064,7 +2073,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>54</v>
       </c>
@@ -2077,7 +2086,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>55</v>
       </c>
@@ -2090,7 +2099,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>56</v>
       </c>
@@ -2103,7 +2112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>57</v>
       </c>
@@ -2118,7 +2127,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>58</v>
       </c>
@@ -2131,7 +2140,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>59</v>
       </c>
@@ -2145,7 +2154,7 @@
       </c>
       <c r="F97" s="2"/>
     </row>
-    <row r="98" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>60</v>
       </c>
@@ -2159,7 +2168,7 @@
       </c>
       <c r="F98" s="2"/>
     </row>
-    <row r="99" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>61</v>
       </c>
@@ -2175,7 +2184,7 @@
       </c>
       <c r="F99" s="2"/>
     </row>
-    <row r="100" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>62</v>
       </c>
@@ -2189,7 +2198,7 @@
       </c>
       <c r="F100" s="2"/>
     </row>
-    <row r="101" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>63</v>
       </c>
@@ -2203,7 +2212,7 @@
       </c>
       <c r="F101" s="2"/>
     </row>
-    <row r="102" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>64</v>
       </c>
@@ -2217,7 +2226,7 @@
       </c>
       <c r="F102" s="2"/>
     </row>
-    <row r="103" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>65</v>
       </c>
@@ -2233,7 +2242,7 @@
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
     </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>66</v>
       </c>
@@ -2247,19 +2256,19 @@
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B105" s="2"/>
       <c r="C105" s="3"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
     </row>
-    <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>67</v>
       </c>
@@ -2276,7 +2285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>68</v>
       </c>
@@ -2292,7 +2301,7 @@
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
     </row>
-    <row r="109" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>69</v>
       </c>
@@ -2308,7 +2317,7 @@
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
     </row>
-    <row r="110" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>70</v>
       </c>
@@ -2324,7 +2333,7 @@
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
     </row>
-    <row r="111" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>71</v>
       </c>
@@ -2340,7 +2349,7 @@
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
     </row>
-    <row r="112" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>72</v>
       </c>
@@ -2356,7 +2365,7 @@
       </c>
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>73</v>
       </c>
@@ -2369,7 +2378,7 @@
       </c>
       <c r="E113" s="2"/>
     </row>
-    <row r="114" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>74</v>
       </c>
@@ -2382,7 +2391,7 @@
       </c>
       <c r="E114" s="2"/>
     </row>
-    <row r="115" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="135" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>75</v>
       </c>
@@ -2395,7 +2404,7 @@
       </c>
       <c r="E115" s="2"/>
     </row>
-    <row r="116" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>76</v>
       </c>
@@ -2410,7 +2419,7 @@
       </c>
       <c r="E116" s="2"/>
     </row>
-    <row r="117" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>77</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>78</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="90" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>79</v>
       </c>
@@ -2461,7 +2470,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>80</v>
       </c>
@@ -2476,7 +2485,7 @@
       </c>
       <c r="E120" s="2"/>
     </row>
-    <row r="121" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>81</v>
       </c>
@@ -2491,7 +2500,7 @@
       </c>
       <c r="E121" s="2"/>
     </row>
-    <row r="122" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="120" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>82</v>
       </c>
@@ -2504,7 +2513,7 @@
       </c>
       <c r="E122" s="2"/>
     </row>
-    <row r="123" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>83</v>
       </c>
@@ -2512,12 +2521,14 @@
         <v>147</v>
       </c>
       <c r="C123" s="3"/>
-      <c r="D123" s="6"/>
+      <c r="D123" s="6">
+        <v>0</v>
+      </c>
       <c r="E123" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>84</v>
       </c>
@@ -2528,7 +2539,7 @@
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
     </row>
-    <row r="125" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>85</v>
       </c>
@@ -2545,7 +2556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>86</v>
       </c>

</xml_diff>